<commit_message>
Brackets Download functionality added.
</commit_message>
<xml_diff>
--- a/TRNMNT/DocSamples/brackets-8.xlsx
+++ b/TRNMNT/DocSamples/brackets-8.xlsx
@@ -19,6 +19,10 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
@@ -34,8 +38,8 @@
     </font>
     <font>
       <sz val="14"/>
-      <name val="Arial Cyr"/>
-      <charset val="204"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -141,14 +145,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,63 +470,71 @@
   <dimension ref="B2:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="I4" sqref="I4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="20.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="27" style="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="20.7109375" style="10" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C2" s="2"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
       <c r="D4" s="2"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C5" s="3"/>
       <c r="D5" s="2"/>
-      <c r="I5" s="4"/>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C6" s="5"/>
       <c r="D6" s="2"/>
-      <c r="I6" s="4"/>
+      <c r="I6" s="11"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="4"/>
+      <c r="I7" s="11"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C8" s="5"/>
       <c r="D8" s="3"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="I8" s="11"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="5"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="9"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="12"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
@@ -533,44 +554,44 @@
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="5"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C15" s="3"/>
       <c r="D15" s="5"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="I15" s="11"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="I16" s="11"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C17" s="5"/>
       <c r="D17" s="8"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="4"/>
+      <c r="I17" s="11"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C18" s="5"/>
-      <c r="I18" s="4"/>
+      <c r="I18" s="11"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C19" s="5"/>
-      <c r="I19" s="4"/>
+      <c r="I19" s="11"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="11"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="9"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="12"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
@@ -594,7 +615,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToWidth="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>